<commit_message>
add last report + ash timesheet update
</commit_message>
<xml_diff>
--- a/timesheets/ash/timesheet_second_semester.xlsx
+++ b/timesheets/ash/timesheet_second_semester.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ash/Desktop/Boulder/Fa23 Classes/canopy/admin/timesheets/ash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A832CFF-2FCD-F84F-AB60-B89BBEC99385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095B9EA9-BB32-2A4D-80EB-DA265BE07294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Week11" sheetId="14" r:id="rId11"/>
     <sheet name="Week12" sheetId="15" r:id="rId12"/>
     <sheet name="Week13" sheetId="16" r:id="rId13"/>
+    <sheet name="Week14" sheetId="17" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -144,6 +145,9 @@
   </si>
   <si>
     <t>tasks much harder than expected :( but almost done!</t>
+  </si>
+  <si>
+    <t>Expo</t>
   </si>
 </sst>
 </file>
@@ -383,6 +387,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,7 +418,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -713,11 +717,11 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -728,11 +732,11 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -752,15 +756,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="B4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1072,11 +1076,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -1087,11 +1091,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -1111,15 +1115,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1499,11 +1503,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -1514,11 +1518,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="33"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -1538,15 +1542,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1903,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AC76FF-E899-704D-B794-64B3C211A090}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1916,11 +1920,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="13" t="s">
         <v>30</v>
       </c>
@@ -1935,11 +1939,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="33"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -1959,15 +1963,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2211,9 +2215,424 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I16" s="35">
+      <c r="I16" s="25">
         <f>SUM(B16:H16)</f>
         <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D50138-78E3-8F40-9F7F-1C393F988A83}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="17">
+        <v>45404</v>
+      </c>
+      <c r="C5" s="17">
+        <v>45405</v>
+      </c>
+      <c r="D5" s="17">
+        <v>45406</v>
+      </c>
+      <c r="E5" s="17">
+        <v>45407</v>
+      </c>
+      <c r="F5" s="17">
+        <v>45408</v>
+      </c>
+      <c r="G5" s="17">
+        <v>45409</v>
+      </c>
+      <c r="H5" s="17">
+        <v>45410</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20">
+        <v>2</v>
+      </c>
+      <c r="I12" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="19">
+        <v>3</v>
+      </c>
+      <c r="C13" s="19">
+        <v>3</v>
+      </c>
+      <c r="D13" s="19">
+        <v>3</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19">
+        <v>6</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4">
+        <f>SUM(B6:B15)</f>
+        <v>4</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:H16" si="0">SUM(C6:C15)</f>
+        <v>3</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="25">
+        <f>SUM(B16:H16)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -2342,11 +2761,11 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -2357,11 +2776,11 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2381,15 +2800,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="B4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2699,11 +3118,11 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -2714,11 +3133,11 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2738,15 +3157,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="B4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3060,11 +3479,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -3076,11 +3495,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -3102,15 +3521,15 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13"/>
       <c r="J4" s="14"/>
     </row>
@@ -3510,11 +3929,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -3525,11 +3944,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -3549,15 +3968,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3930,11 +4349,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -3945,11 +4364,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -3969,15 +4388,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4352,11 +4771,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -4367,11 +4786,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -4391,15 +4810,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4772,11 +5191,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -4787,11 +5206,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -4811,15 +5230,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5194,11 +5613,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -5209,11 +5628,11 @@
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -5233,15 +5652,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>